<commit_message>
[ADD] new parameters set
</commit_message>
<xml_diff>
--- a/parameters/RS11.xlsx
+++ b/parameters/RS11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Desktop\TIA\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6288D07F-E231-40E9-8E68-9EFB585C1615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B09448A-EFF8-4B1B-AD05-EF82C0198AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2535" yWindow="2265" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +128,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,13 +225,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
@@ -508,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +545,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
@@ -551,7 +560,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>1.67</v>
+        <v>4.33</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
@@ -566,10 +575,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>3.8</v>
+        <v>1.98</v>
       </c>
       <c r="C4" s="3">
-        <v>3.8</v>
+        <v>1.98</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -634,10 +643,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="3">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="C8" s="3">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>20</v>
@@ -646,7 +655,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>